<commit_message>
Update tests. New xlsx file for testSearch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876F9E9D-48E8-4632-A6D9-7D3EE3FB957F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,36 +20,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>SearchData</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>j</t>
+    <t>Your Objective</t>
+  </si>
+  <si>
+    <t>Heder</t>
+  </si>
+  <si>
+    <t>Achieve your goal</t>
+  </si>
+  <si>
+    <t>Choose your pack</t>
+  </si>
+  <si>
+    <t>Pricing</t>
+  </si>
+  <si>
+    <t>IT-Platforma</t>
+  </si>
+  <si>
+    <t>Robert'); DROP TABLE Students;--</t>
+  </si>
+  <si>
+    <t>XSS</t>
+  </si>
+  <si>
+    <t>Nice site,  I think I'll take it.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,7 +92,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,20 +369,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -383,63 +391,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>